<commit_message>
Changed syntax to match Codebook variable name suggestions
</commit_message>
<xml_diff>
--- a/Matrice_intermediaire.xlsx
+++ b/Matrice_intermediaire.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
-    <t xml:space="preserve">adm1_name</t>
+    <t xml:space="preserve">ADMIN1Name</t>
   </si>
   <si>
-    <t xml:space="preserve">adm2_name</t>
+    <t xml:space="preserve">ADMIN2Name</t>
   </si>
   <si>
     <t xml:space="preserve">Population</t>
@@ -74,19 +74,19 @@
     <t xml:space="preserve">HHS_finalphase</t>
   </si>
   <si>
-    <t xml:space="preserve">LHCS_NoStrategies</t>
+    <t xml:space="preserve">LhHCSCat_NoStrategies</t>
   </si>
   <si>
-    <t xml:space="preserve">LHCS_StressStrategies</t>
+    <t xml:space="preserve">LhHCSCat_StressStrategies</t>
   </si>
   <si>
-    <t xml:space="preserve">LHCS_CrisisStategies</t>
+    <t xml:space="preserve">LhHCSCat_CrisisStategies</t>
   </si>
   <si>
-    <t xml:space="preserve">LHCS_EmergencyStrategies</t>
+    <t xml:space="preserve">LhHCSCat_EmergencyStrategies</t>
   </si>
   <si>
-    <t xml:space="preserve">LHCS_finalphase</t>
+    <t xml:space="preserve">LhHCSCat_finalphase</t>
   </si>
   <si>
     <t xml:space="preserve">rCSI_Phase1</t>

</xml_diff>